<commit_message>
updated readme and model3 file
</commit_message>
<xml_diff>
--- a/model_graphs/model3_bargraph.xlsx
+++ b/model_graphs/model3_bargraph.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelrogo/software/cli_he_code/hacked/notebooks/model_data/mymodel/avian_Flu/tuned_model/paperAnalysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelrogo/software/cli_he_code/paper/nature_coms/coms/model_graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1941C1-95D2-7341-B6C0-FF05B43A44DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8650151-E540-C24A-BD2B-D70111BC667C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5860" yWindow="3200" windowWidth="27240" windowHeight="14800" xr2:uid="{7E983D7B-FAD3-B747-B5A6-696F61638F70}"/>
+    <workbookView xWindow="1560" yWindow="1500" windowWidth="27240" windowHeight="14800" xr2:uid="{7E983D7B-FAD3-B747-B5A6-696F61638F70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,7 +472,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>22.670352173716271</v>
@@ -480,7 +480,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8">
         <v>23.956294639654683</v>

</xml_diff>